<commit_message>
Added Serial Number upload
</commit_message>
<xml_diff>
--- a/QBD2/wwwroot/upload/80000019001A7.xlsx
+++ b/QBD2/wwwroot/upload/80000019001A7.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/dc25c420738c9e7d/PPG/Projects/LightspeedAviation/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="3" documentId="8_{E9A1F884-34D5-4CF2-8CAB-8409F4B19CD4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{C1AE241B-33A9-4296-A80D-FA85EAB1B134}"/>
+  <xr:revisionPtr revIDLastSave="5" documentId="8_{E9A1F884-34D5-4CF2-8CAB-8409F4B19CD4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{735DA457-B855-47E3-9EBE-8E89769129AA}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{126F16D0-1DAC-492C-8092-71CAC1D9DB91}"/>
+    <workbookView xWindow="3510" yWindow="3510" windowWidth="21600" windowHeight="11385" xr2:uid="{126F16D0-1DAC-492C-8092-71CAC1D9DB91}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -387,10 +387,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A2F8BDAA-06FE-43EE-BE79-DB833F46F6E6}">
-  <dimension ref="A1:A11"/>
+  <dimension ref="A1:A12"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A3" sqref="A3"/>
+      <selection activeCell="A12" sqref="A12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -453,6 +453,11 @@
         <v>100127759</v>
       </c>
     </row>
+    <row r="12" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A12">
+        <v>333333333333</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>